<commit_message>
Update Meteora Ecommerce - AULA INICIAL.xlsx
</commit_message>
<xml_diff>
--- a/Alura-Automação/Meteora Ecommerce - AULA INICIAL.xlsx
+++ b/Alura-Automação/Meteora Ecommerce - AULA INICIAL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://officeresolve-my.sharepoint.com/personal/r_sabino_officeresolve_com_br/Documents/Alura-Ciência de Dados/02 - Excel - Novas Formações/Formação Excel/3197 - Excel  3 - Recursos Visuais Gráficos e Formatos/Materiais do Curso/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danie\OneDrive\Documentos\GitHub\Alura-Automa--o\Alura-Automação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{FAC21677-FA40-4B71-A1A0-282C39E9EB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6927879-564D-4525-A66D-F8936B511DA5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{15BDFDBD-4866-4550-B853-2E70A0E19785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11040" firstSheet="2" activeTab="2" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="2" xr2:uid="{F6D97A53-F63B-4272-A181-44B26E0B790F}"/>
   </bookViews>
   <sheets>
     <sheet name="Meu Gráfico" sheetId="6" state="hidden" r:id="rId1"/>
@@ -27,31 +27,20 @@
     <definedName name="Int_Nome_Produtos">#REF!</definedName>
     <definedName name="Int_Quantidade">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="90">
   <si>
     <t>Produtos</t>
   </si>
@@ -318,6 +307,9 @@
   </si>
   <si>
     <t>Estoque</t>
+  </si>
+  <si>
+    <t>Situação</t>
   </si>
 </sst>
 </file>
@@ -788,7 +780,57 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título Meteora" xfId="2" xr:uid="{52F1EA3C-B23E-4AE6-AE73-27AD9F7C9021}"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2110,7 +2152,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Office Resolve Testes" refreshedDate="45091.695904398148" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="39" xr:uid="{D9D057AD-0FAE-4908-B186-309A9CA94BEA}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A3:G42" sheet="Produtos"/>
+    <worksheetSource ref="A3:H42" sheet="Produtos"/>
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="Produtos" numFmtId="0">
@@ -2525,7 +2567,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{37A4C077-C9C3-4E33-8B3E-9194B9F750DF}" name="Tabela dinâmica85" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{37A4C077-C9C3-4E33-8B3E-9194B9F750DF}" name="Tabela dinâmica85" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -2693,36 +2735,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40AC111B-A369-4C0B-9503-7C5B9442DAEA}" name="TB_Produtos" displayName="TB_Produtos" ref="A3:F42" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="A3:F42" xr:uid="{40AC111B-A369-4C0B-9503-7C5B9442DAEA}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40AC111B-A369-4C0B-9503-7C5B9442DAEA}" name="TB_Produtos" displayName="TB_Produtos" ref="A3:G42" totalsRowShown="0" headerRowDxfId="19">
+  <autoFilter ref="A3:G42" xr:uid="{40AC111B-A369-4C0B-9503-7C5B9442DAEA}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{2F8ED5FF-48A1-488E-9DF1-FE060F71A415}" name="Código"/>
     <tableColumn id="2" xr3:uid="{E100D4E2-C3A0-43FF-A1D9-90A4BC2A9918}" name="Produtos"/>
-    <tableColumn id="3" xr3:uid="{2EF7FEE0-6B6F-4534-86A0-46B6555B7BEF}" name="Tamanho" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{2EF7FEE0-6B6F-4534-86A0-46B6555B7BEF}" name="Tamanho" dataDxfId="18"/>
     <tableColumn id="4" xr3:uid="{4435A4B8-E7F0-4D66-A4F8-6A9FEAA36D5A}" name="Categoria"/>
-    <tableColumn id="6" xr3:uid="{15F9CACC-A558-4A20-80CF-C2ADA2603221}" name="Estoque" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{CA8AD0DE-58EC-4839-85FB-1DD75DA28087}" name="Preço Unitário" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{15F9CACC-A558-4A20-80CF-C2ADA2603221}" name="Estoque" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{47341692-C6E3-4D07-A99B-C56805CF57DF}" name="Situação" dataDxfId="4">
+      <calculatedColumnFormula>TB_Produtos[[#This Row],[Estoque]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{CA8AD0DE-58EC-4839-85FB-1DD75DA28087}" name="Preço Unitário" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AD739091-30BD-4C30-BDDA-7504C0C4B6E2}" name="TB_Vendas" displayName="TB_Vendas" ref="A2:H61" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" headerRowCellStyle="Cabeçalho Meteora">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AD739091-30BD-4C30-BDDA-7504C0C4B6E2}" name="TB_Vendas" displayName="TB_Vendas" ref="A2:H61" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowCellStyle="Cabeçalho Meteora">
   <autoFilter ref="A2:H61" xr:uid="{AD739091-30BD-4C30-BDDA-7504C0C4B6E2}"/>
   <tableColumns count="8">
-    <tableColumn id="7" xr3:uid="{5E8DE7C3-CDB6-4314-A5CC-C44D3C21973F}" name="Mês" dataDxfId="8">
+    <tableColumn id="7" xr3:uid="{5E8DE7C3-CDB6-4314-A5CC-C44D3C21973F}" name="Mês" dataDxfId="13">
       <calculatedColumnFormula>MONTH(TB_Vendas[[#This Row],[Data]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{43632F1F-6978-4CE7-BB13-7CCE587D6821}" name="Data" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{49DF5362-33BE-4541-BD47-0B512249381E}" name="Código" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{B3C718A1-FEFF-4C65-9CA1-DF94EF755918}" name="Tamanho" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{43632F1F-6978-4CE7-BB13-7CCE587D6821}" name="Data" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{49DF5362-33BE-4541-BD47-0B512249381E}" name="Código" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{B3C718A1-FEFF-4C65-9CA1-DF94EF755918}" name="Tamanho" dataDxfId="10">
       <calculatedColumnFormula>_xlfn.XLOOKUP(C3,TB_Produtos[Código],TB_Produtos[Tamanho])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1F3EAF93-84E7-4086-BE54-3AB7D71B21A8}" name="Categoria" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{7DC2ADED-AF8A-4BC8-A38E-FEF676FE49C9}" name="Qtd" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{9459B662-6A4F-4486-82B1-12F67B8F842E}" name="Total" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{192FEBCA-1287-48A6-9BE6-69528F71C305}" name="Vendedor" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{1F3EAF93-84E7-4086-BE54-3AB7D71B21A8}" name="Categoria" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{7DC2ADED-AF8A-4BC8-A38E-FEF676FE49C9}" name="Qtd" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{9459B662-6A4F-4486-82B1-12F67B8F842E}" name="Total" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{192FEBCA-1287-48A6-9BE6-69528F71C305}" name="Vendedor" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3031,13 +3076,13 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
@@ -3045,7 +3090,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -3053,7 +3098,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3061,7 +3106,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3069,7 +3114,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -3077,7 +3122,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -3085,7 +3130,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -3093,7 +3138,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -3101,7 +3146,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -3109,7 +3154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -3117,7 +3162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -3125,7 +3170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -3133,7 +3178,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -3141,7 +3186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -3149,7 +3194,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -3157,7 +3202,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -3165,7 +3210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -3173,7 +3218,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -3181,7 +3226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -3196,23 +3241,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8ADA2D8-DE9E-4ACF-B5A7-8907124C5CF1}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="33" t="s">
         <v>15</v>
       </c>
@@ -3221,16 +3270,18 @@
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
       <c r="F1" s="33"/>
-    </row>
-    <row r="2" spans="1:6" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G1" s="33"/>
+    </row>
+    <row r="2" spans="1:7" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>41</v>
       </c>
@@ -3247,10 +3298,13 @@
         <v>88</v>
       </c>
       <c r="F3" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3266,11 +3320,15 @@
       <c r="E4" s="1">
         <v>12</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>12</v>
+      </c>
+      <c r="G4" s="28">
         <v>65.900000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -3286,11 +3344,15 @@
       <c r="E5" s="1">
         <v>15</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>15</v>
+      </c>
+      <c r="G5" s="28">
         <v>69.900000000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -3306,11 +3368,15 @@
       <c r="E6" s="1">
         <v>5</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G6" s="28">
         <v>70.900000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -3326,11 +3392,15 @@
       <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>2</v>
+      </c>
+      <c r="G7" s="28">
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -3346,11 +3416,15 @@
       <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="28">
         <v>259.89999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -3366,11 +3440,15 @@
       <c r="E9" s="1">
         <v>11</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>11</v>
+      </c>
+      <c r="G9" s="28">
         <v>39.9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -3386,11 +3464,15 @@
       <c r="E10" s="1">
         <v>6</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>6</v>
+      </c>
+      <c r="G10" s="28">
         <v>85.9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -3406,11 +3488,15 @@
       <c r="E11" s="1">
         <v>5</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G11" s="28">
         <v>89.9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -3426,11 +3512,15 @@
       <c r="E12" s="1">
         <v>8</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>8</v>
+      </c>
+      <c r="G12" s="28">
         <v>92.9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -3446,11 +3536,15 @@
       <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>2</v>
+      </c>
+      <c r="G13" s="28">
         <v>44.9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -3466,11 +3560,15 @@
       <c r="E14" s="1">
         <v>3</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>3</v>
+      </c>
+      <c r="G14" s="28">
         <v>46.9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -3486,11 +3584,15 @@
       <c r="E15" s="1">
         <v>5</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F15" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G15" s="28">
         <v>48.9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -3506,11 +3608,15 @@
       <c r="E16" s="1">
         <v>6</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>6</v>
+      </c>
+      <c r="G16" s="28">
         <v>39.9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -3526,11 +3632,15 @@
       <c r="E17" s="1">
         <v>10</v>
       </c>
-      <c r="F17" s="28">
+      <c r="F17" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>10</v>
+      </c>
+      <c r="G17" s="28">
         <v>39.9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -3546,11 +3656,15 @@
       <c r="E18" s="1">
         <v>12</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F18" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>12</v>
+      </c>
+      <c r="G18" s="28">
         <v>42.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -3566,11 +3680,15 @@
       <c r="E19" s="1">
         <v>6</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>6</v>
+      </c>
+      <c r="G19" s="28">
         <v>25.9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -3586,11 +3704,15 @@
       <c r="E20" s="1">
         <v>10</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>10</v>
+      </c>
+      <c r="G20" s="28">
         <v>29.9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -3606,11 +3728,15 @@
       <c r="E21" s="1">
         <v>12</v>
       </c>
-      <c r="F21" s="28">
+      <c r="F21" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>12</v>
+      </c>
+      <c r="G21" s="28">
         <v>32.9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -3626,11 +3752,15 @@
       <c r="E22" s="1">
         <v>21</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F22" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>21</v>
+      </c>
+      <c r="G22" s="28">
         <v>49.9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -3646,11 +3776,15 @@
       <c r="E23" s="1">
         <v>5</v>
       </c>
-      <c r="F23" s="28">
+      <c r="F23" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G23" s="28">
         <v>299.89999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -3666,11 +3800,15 @@
       <c r="E24" s="1">
         <v>5</v>
       </c>
-      <c r="F24" s="28">
+      <c r="F24" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G24" s="28">
         <v>302.89999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -3686,11 +3824,15 @@
       <c r="E25" s="1">
         <v>5</v>
       </c>
-      <c r="F25" s="28">
+      <c r="F25" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G25" s="28">
         <v>300</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -3706,11 +3848,15 @@
       <c r="E26" s="1">
         <v>5</v>
       </c>
-      <c r="F26" s="28">
+      <c r="F26" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G26" s="28">
         <v>249.9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -3726,11 +3872,15 @@
       <c r="E27" s="1">
         <v>5</v>
       </c>
-      <c r="F27" s="28">
+      <c r="F27" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G27" s="28">
         <v>259.89999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -3746,11 +3896,15 @@
       <c r="E28" s="1">
         <v>5</v>
       </c>
-      <c r="F28" s="28">
+      <c r="F28" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G28" s="28">
         <v>299.89999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -3766,11 +3920,15 @@
       <c r="E29" s="1">
         <v>3</v>
       </c>
-      <c r="F29" s="28">
+      <c r="F29" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>3</v>
+      </c>
+      <c r="G29" s="28">
         <v>349.9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -3786,11 +3944,15 @@
       <c r="E30" s="1">
         <v>3</v>
       </c>
-      <c r="F30" s="28">
+      <c r="F30" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>3</v>
+      </c>
+      <c r="G30" s="28">
         <v>399.9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -3806,11 +3968,15 @@
       <c r="E31" s="1">
         <v>5</v>
       </c>
-      <c r="F31" s="28">
+      <c r="F31" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G31" s="28">
         <v>249.9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -3826,11 +3992,15 @@
       <c r="E32" s="1">
         <v>3</v>
       </c>
-      <c r="F32" s="28">
+      <c r="F32" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>3</v>
+      </c>
+      <c r="G32" s="28">
         <v>255</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -3846,11 +4016,15 @@
       <c r="E33" s="1">
         <v>5</v>
       </c>
-      <c r="F33" s="28">
+      <c r="F33" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G33" s="28">
         <v>259.89999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -3866,11 +4040,15 @@
       <c r="E34" s="1">
         <v>5</v>
       </c>
-      <c r="F34" s="28">
+      <c r="F34" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G34" s="28">
         <v>199.9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -3886,11 +4064,15 @@
       <c r="E35" s="1">
         <v>5</v>
       </c>
-      <c r="F35" s="28">
+      <c r="F35" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G35" s="28">
         <v>249.9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>75</v>
       </c>
@@ -3906,11 +4088,15 @@
       <c r="E36" s="1">
         <v>5</v>
       </c>
-      <c r="F36" s="28">
+      <c r="F36" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>5</v>
+      </c>
+      <c r="G36" s="28">
         <v>259.89999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>76</v>
       </c>
@@ -3926,11 +4112,15 @@
       <c r="E37" s="1">
         <v>3</v>
       </c>
-      <c r="F37" s="28">
+      <c r="F37" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>3</v>
+      </c>
+      <c r="G37" s="28">
         <v>89.9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -3946,11 +4136,15 @@
       <c r="E38" s="1">
         <v>3</v>
       </c>
-      <c r="F38" s="28">
+      <c r="F38" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>3</v>
+      </c>
+      <c r="G38" s="28">
         <v>91.4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -3966,11 +4160,15 @@
       <c r="E39" s="1">
         <v>3</v>
       </c>
-      <c r="F39" s="28">
+      <c r="F39" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>3</v>
+      </c>
+      <c r="G39" s="28">
         <v>93.5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -3986,11 +4184,15 @@
       <c r="E40" s="1">
         <v>2</v>
       </c>
-      <c r="F40" s="28">
+      <c r="F40" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>2</v>
+      </c>
+      <c r="G40" s="28">
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -4006,11 +4208,15 @@
       <c r="E41" s="1">
         <v>2</v>
       </c>
-      <c r="F41" s="28">
+      <c r="F41" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>2</v>
+      </c>
+      <c r="G41" s="28">
         <v>142.9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -4026,18 +4232,65 @@
       <c r="E42" s="1">
         <v>2</v>
       </c>
-      <c r="F42" s="28">
+      <c r="F42" s="1">
+        <f>TB_Produtos[[#This Row],[Estoque]]</f>
+        <v>2</v>
+      </c>
+      <c r="G42" s="28">
         <v>146</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
+  <conditionalFormatting sqref="F4:F42">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Symbols" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="percent" val="10" gte="0"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G42">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFDAFF01"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D60DF3B7-7EF8-4AA8-ABA4-31894846E9FA}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D60DF3B7-7EF8-4AA8-ABA4-31894846E9FA}">
+            <x14:dataBar minLength="0" maxLength="100" direction="rightToLeft">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G4:G42</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4049,19 +4302,19 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="33" t="s">
         <v>15</v>
       </c>
@@ -4073,7 +4326,7 @@
       <c r="G1" s="33"/>
       <c r="H1" s="33"/>
     </row>
-    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>42</v>
       </c>
@@ -4099,7 +4352,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>1</v>
@@ -4110,9 +4363,9 @@
       <c r="C3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C3,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>Único</v>
+      <c r="D3" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C3,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
@@ -4127,7 +4380,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>1</v>
@@ -4138,9 +4391,9 @@
       <c r="C4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="1">
-        <f>_xlfn.XLOOKUP(C4,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>36</v>
+      <c r="D4" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C4,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>82</v>
@@ -4155,7 +4408,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>1</v>
@@ -4166,9 +4419,9 @@
       <c r="C5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="1">
-        <f>_xlfn.XLOOKUP(C5,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>37</v>
+      <c r="D5" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C5,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>82</v>
@@ -4183,7 +4436,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>1</v>
@@ -4194,9 +4447,9 @@
       <c r="C6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C6,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D6" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C6,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
@@ -4211,7 +4464,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>1</v>
@@ -4222,9 +4475,9 @@
       <c r="C7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C7,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D7" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C7,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>12</v>
@@ -4239,7 +4492,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>1</v>
@@ -4250,9 +4503,9 @@
       <c r="C8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="1">
-        <f>_xlfn.XLOOKUP(C8,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>36</v>
+      <c r="D8" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C8,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>82</v>
@@ -4267,7 +4520,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>1</v>
@@ -4278,9 +4531,9 @@
       <c r="C9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C9,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>Único</v>
+      <c r="D9" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C9,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>13</v>
@@ -4295,7 +4548,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>1</v>
@@ -4306,9 +4559,9 @@
       <c r="C10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C10,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D10" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C10,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>12</v>
@@ -4323,7 +4576,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>1</v>
@@ -4334,9 +4587,9 @@
       <c r="C11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C11,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D11" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C11,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>12</v>
@@ -4351,7 +4604,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>1</v>
@@ -4362,9 +4615,9 @@
       <c r="C12" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C12,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D12" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C12,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
@@ -4379,7 +4632,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>1</v>
@@ -4390,9 +4643,9 @@
       <c r="C13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C13,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D13" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C13,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
@@ -4407,7 +4660,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>2</v>
@@ -4418,9 +4671,9 @@
       <c r="C14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C14,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>Único</v>
+      <c r="D14" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C14,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>13</v>
@@ -4435,7 +4688,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>2</v>
@@ -4446,9 +4699,9 @@
       <c r="C15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C15,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>P</v>
+      <c r="D15" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C15,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>12</v>
@@ -4463,7 +4716,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>2</v>
@@ -4474,9 +4727,9 @@
       <c r="C16" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="1">
-        <f>_xlfn.XLOOKUP(C16,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>37</v>
+      <c r="D16" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C16,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>82</v>
@@ -4491,7 +4744,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>2</v>
@@ -4502,9 +4755,9 @@
       <c r="C17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C17,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D17" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C17,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>12</v>
@@ -4519,7 +4772,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>2</v>
@@ -4530,9 +4783,9 @@
       <c r="C18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="1">
-        <f>_xlfn.XLOOKUP(C18,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>38</v>
+      <c r="D18" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C18,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>82</v>
@@ -4547,7 +4800,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>2</v>
@@ -4558,9 +4811,9 @@
       <c r="C19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C19,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>P</v>
+      <c r="D19" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C19,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>12</v>
@@ -4575,7 +4828,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>2</v>
@@ -4586,9 +4839,9 @@
       <c r="C20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C20,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D20" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C20,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>12</v>
@@ -4603,7 +4856,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>3</v>
@@ -4614,9 +4867,9 @@
       <c r="C21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C21,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D21" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C21,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>12</v>
@@ -4631,7 +4884,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>3</v>
@@ -4642,9 +4895,9 @@
       <c r="C22" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="1">
-        <f>_xlfn.XLOOKUP(C22,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>37</v>
+      <c r="D22" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C22,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>82</v>
@@ -4659,7 +4912,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>3</v>
@@ -4670,9 +4923,9 @@
       <c r="C23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C23,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>Único</v>
+      <c r="D23" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C23,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>13</v>
@@ -4687,7 +4940,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>3</v>
@@ -4698,9 +4951,9 @@
       <c r="C24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C24,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D24" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C24,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>12</v>
@@ -4715,7 +4968,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>3</v>
@@ -4726,9 +4979,9 @@
       <c r="C25" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C25,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D25" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C25,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>12</v>
@@ -4743,7 +4996,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>3</v>
@@ -4754,9 +5007,9 @@
       <c r="C26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C26,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D26" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C26,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>12</v>
@@ -4771,7 +5024,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>3</v>
@@ -4782,9 +5035,9 @@
       <c r="C27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="1">
-        <f>_xlfn.XLOOKUP(C27,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>37</v>
+      <c r="D27" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C27,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>82</v>
@@ -4799,7 +5052,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>3</v>
@@ -4810,9 +5063,9 @@
       <c r="C28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C28,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D28" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C28,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>12</v>
@@ -4827,7 +5080,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>3</v>
@@ -4838,9 +5091,9 @@
       <c r="C29" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="1">
-        <f>_xlfn.XLOOKUP(C29,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>37</v>
+      <c r="D29" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C29,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>82</v>
@@ -4855,7 +5108,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>3</v>
@@ -4866,9 +5119,9 @@
       <c r="C30" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C30,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D30" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C30,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>12</v>
@@ -4883,7 +5136,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>4</v>
@@ -4894,9 +5147,9 @@
       <c r="C31" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C31,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D31" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C31,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>12</v>
@@ -4911,7 +5164,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>4</v>
@@ -4922,9 +5175,9 @@
       <c r="C32" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="1">
-        <f>_xlfn.XLOOKUP(C32,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>36</v>
+      <c r="D32" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C32,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>82</v>
@@ -4939,7 +5192,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>4</v>
@@ -4950,9 +5203,9 @@
       <c r="C33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D33" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C33,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D33" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C33,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>12</v>
@@ -4967,7 +5220,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>4</v>
@@ -4978,9 +5231,9 @@
       <c r="C34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C34,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>P</v>
+      <c r="D34" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C34,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>12</v>
@@ -4995,7 +5248,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>4</v>
@@ -5006,9 +5259,9 @@
       <c r="C35" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C35,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D35" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C35,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>12</v>
@@ -5023,7 +5276,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>4</v>
@@ -5034,9 +5287,9 @@
       <c r="C36" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C36,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>P</v>
+      <c r="D36" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C36,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>12</v>
@@ -5051,7 +5304,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>4</v>
@@ -5062,9 +5315,9 @@
       <c r="C37" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C37,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D37" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C37,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>12</v>
@@ -5079,7 +5332,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>4</v>
@@ -5090,9 +5343,9 @@
       <c r="C38" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C38,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D38" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C38,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>12</v>
@@ -5107,7 +5360,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>4</v>
@@ -5118,9 +5371,9 @@
       <c r="C39" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D39" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C39,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D39" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C39,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>12</v>
@@ -5135,7 +5388,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>4</v>
@@ -5146,9 +5399,9 @@
       <c r="C40" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C40,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D40" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C40,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>12</v>
@@ -5163,7 +5416,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>4</v>
@@ -5174,9 +5427,9 @@
       <c r="C41" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C41,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D41" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C41,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>12</v>
@@ -5191,7 +5444,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>5</v>
@@ -5202,9 +5455,9 @@
       <c r="C42" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C42,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D42" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C42,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>12</v>
@@ -5219,7 +5472,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>5</v>
@@ -5230,9 +5483,9 @@
       <c r="C43" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C43,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D43" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C43,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>12</v>
@@ -5247,7 +5500,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>5</v>
@@ -5258,9 +5511,9 @@
       <c r="C44" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D44" s="1">
-        <f>_xlfn.XLOOKUP(C44,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>37</v>
+      <c r="D44" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C44,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>82</v>
@@ -5275,7 +5528,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>5</v>
@@ -5286,9 +5539,9 @@
       <c r="C45" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D45" s="1">
-        <f>_xlfn.XLOOKUP(C45,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>37</v>
+      <c r="D45" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C45,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>82</v>
@@ -5303,7 +5556,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>5</v>
@@ -5314,9 +5567,9 @@
       <c r="C46" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D46" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C46,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D46" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C46,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>12</v>
@@ -5331,7 +5584,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>5</v>
@@ -5342,9 +5595,9 @@
       <c r="C47" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D47" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C47,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>Único</v>
+      <c r="D47" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C47,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>13</v>
@@ -5359,7 +5612,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>5</v>
@@ -5370,9 +5623,9 @@
       <c r="C48" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D48" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C48,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D48" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C48,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>12</v>
@@ -5387,7 +5640,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>6</v>
@@ -5398,9 +5651,9 @@
       <c r="C49" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D49" s="1">
-        <f>_xlfn.XLOOKUP(C49,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>36</v>
+      <c r="D49" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C49,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>82</v>
@@ -5415,7 +5668,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>6</v>
@@ -5426,9 +5679,9 @@
       <c r="C50" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D50" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C50,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D50" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C50,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>12</v>
@@ -5443,7 +5696,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>6</v>
@@ -5454,9 +5707,9 @@
       <c r="C51" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D51" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C51,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>Único</v>
+      <c r="D51" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C51,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>13</v>
@@ -5471,7 +5724,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>6</v>
@@ -5482,9 +5735,9 @@
       <c r="C52" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D52" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C52,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D52" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C52,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>12</v>
@@ -5499,7 +5752,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>6</v>
@@ -5510,9 +5763,9 @@
       <c r="C53" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D53" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C53,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>Único</v>
+      <c r="D53" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C53,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>13</v>
@@ -5527,7 +5780,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>6</v>
@@ -5538,9 +5791,9 @@
       <c r="C54" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D54" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C54,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D54" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C54,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>12</v>
@@ -5555,7 +5808,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>6</v>
@@ -5566,9 +5819,9 @@
       <c r="C55" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D55" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C55,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D55" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C55,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>12</v>
@@ -5583,7 +5836,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>6</v>
@@ -5594,9 +5847,9 @@
       <c r="C56" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D56" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C56,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>G</v>
+      <c r="D56" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C56,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>12</v>
@@ -5611,7 +5864,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>6</v>
@@ -5622,9 +5875,9 @@
       <c r="C57" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D57" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C57,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>Único</v>
+      <c r="D57" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C57,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>13</v>
@@ -5639,7 +5892,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>6</v>
@@ -5650,9 +5903,9 @@
       <c r="C58" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D58" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C58,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D58" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C58,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>12</v>
@@ -5667,7 +5920,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>6</v>
@@ -5678,9 +5931,9 @@
       <c r="C59" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D59" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C59,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>M</v>
+      <c r="D59" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C59,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>12</v>
@@ -5695,7 +5948,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>6</v>
@@ -5706,9 +5959,9 @@
       <c r="C60" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D60" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C60,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>P</v>
+      <c r="D60" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C60,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>12</v>
@@ -5723,7 +5976,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="31">
         <f>MONTH(TB_Vendas[[#This Row],[Data]])</f>
         <v>6</v>
@@ -5734,9 +5987,9 @@
       <c r="C61" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D61" s="1" t="str">
-        <f>_xlfn.XLOOKUP(C61,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
-        <v>Único</v>
+      <c r="D61" s="1" t="e">
+        <f ca="1">_xlfn.XLOOKUP(C61,TB_Produtos[Código],TB_Produtos[Tamanho])</f>
+        <v>#NAME?</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>13</v>
@@ -5756,7 +6009,7 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5787,14 +6040,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="21.33203125" customWidth="1"/>
+    <col min="2" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="8" width="21.33203125" customWidth="1"/>
+    <col min="6" max="8" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="23" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:8" s="23" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="34" t="s">
         <v>36</v>
       </c>
@@ -5806,7 +6059,7 @@
       <c r="G1" s="34"/>
       <c r="H1" s="34"/>
     </row>
-    <row r="2" spans="1:8" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="35" t="s">
         <v>39</v>
       </c>
@@ -5818,7 +6071,7 @@
       <c r="G2" s="36"/>
       <c r="H2" s="37"/>
     </row>
-    <row r="3" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
         <v>37</v>
       </c>
@@ -5838,7 +6091,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="24" t="e">
         <f>COUNTIF(#REF!,"&gt;0")</f>
         <v>#REF!</v>
@@ -5887,18 +6140,18 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="22" t="s">
         <v>1</v>
       </c>
@@ -5906,7 +6159,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
@@ -5914,8 +6167,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="12" t="s">
         <v>0</v>
       </c>
@@ -5938,7 +6191,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>27</v>
       </c>
@@ -5961,7 +6214,7 @@
         <v>501.65999999999997</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
         <v>30</v>
       </c>
@@ -5984,7 +6237,7 @@
         <v>88.02</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
         <v>22</v>
       </c>
@@ -6007,7 +6260,7 @@
         <v>229.5</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
@@ -6030,7 +6283,7 @@
         <v>177.66</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>26</v>
       </c>
@@ -6053,7 +6306,7 @@
         <v>269.90999999999997</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>25</v>
       </c>
@@ -6076,7 +6329,7 @@
         <v>269.90999999999997</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>29</v>
       </c>
@@ -6099,7 +6352,7 @@
         <v>168.3</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>28</v>
       </c>

</xml_diff>